<commit_message>
Updated Scrum Board.xlsx Updated Sprint Backlog.xlsx
</commit_message>
<xml_diff>
--- a/Phase 1/Sprint1/Sprint Backlog.xlsx
+++ b/Phase 1/Sprint1/Sprint Backlog.xlsx
@@ -43,13 +43,13 @@
     <t>Clone project (Inácio)</t>
   </si>
   <si>
-    <t>Bernardo's code smells (Francisco)</t>
-  </si>
-  <si>
-    <t>Bernardo's design patterns (Francisco)</t>
-  </si>
-  <si>
-    <t>Carlos' code smells</t>
+    <t>Bernardo's code smells</t>
+  </si>
+  <si>
+    <t>Bernardo's design patterns</t>
+  </si>
+  <si>
+    <t>Carlos' code smells (Martin)</t>
   </si>
   <si>
     <t>Carlos' design patterns</t>
@@ -64,10 +64,10 @@
     <t>Inacio's code smells</t>
   </si>
   <si>
-    <t>Inacio's design patterns</t>
-  </si>
-  <si>
-    <t>Franciso's code smells</t>
+    <t>Inacio's design patterns (Carlos)</t>
+  </si>
+  <si>
+    <t>Francisco's code smells ( Bernardo)</t>
   </si>
   <si>
     <t>Francisco's design patterns</t>
@@ -122,24 +122,39 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -367,208 +382,259 @@
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="J2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
     <row r="3">
-      <c r="B3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="I3" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="H3" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="J3" s="6"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4">
-      <c r="B4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="I4" s="5" t="s">
+      <c r="B4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="H4" s="9" t="s">
         <v>5</v>
       </c>
+      <c r="J4" s="6"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5">
-      <c r="B5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="I5" s="3" t="s">
+      <c r="B5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="H5" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="J5" s="6"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
     </row>
     <row r="6">
-      <c r="B6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="I6" s="5" t="s">
+      <c r="B6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="F6" s="8"/>
+      <c r="H6" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="J6" s="6"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
     </row>
     <row r="7">
-      <c r="B7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="F7" s="2"/>
-      <c r="I7" s="3" t="s">
+      <c r="B7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="H7" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="J7" s="6"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="D8" s="7"/>
+      <c r="F8" s="8"/>
+      <c r="H8" s="7"/>
+      <c r="J8" s="10"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9">
-      <c r="B9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="F9" s="3" t="s">
+      <c r="B9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="F9" s="4"/>
+      <c r="H9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="J9" s="6"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
     </row>
     <row r="10">
-      <c r="B10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="F10" s="5" t="s">
+      <c r="B10" s="7"/>
+      <c r="D10" s="9"/>
+      <c r="F10" s="8"/>
+      <c r="H10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="J10" s="6"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
     </row>
     <row r="11">
-      <c r="B11" s="3"/>
-      <c r="D11" s="3" t="s">
+      <c r="B11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="F11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="H11" s="3"/>
+      <c r="J11" s="10"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
     </row>
     <row r="12">
-      <c r="B12" s="5"/>
-      <c r="D12" s="5" t="s">
+      <c r="B12" s="9"/>
+      <c r="D12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="F12" s="8"/>
+      <c r="H12" s="7"/>
+      <c r="J12" s="10"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
     </row>
     <row r="13">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="5"/>
+      <c r="D13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="F13" s="4"/>
+      <c r="H13" s="3"/>
+      <c r="J13" s="10"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
     </row>
     <row r="14">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="9"/>
+      <c r="D14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="F14" s="8"/>
+      <c r="H14" s="7"/>
+      <c r="J14" s="10"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
     </row>
     <row r="15">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="5"/>
+      <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="F15" s="4"/>
+      <c r="H15" s="3"/>
+      <c r="J15" s="10"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
     </row>
     <row r="16">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="F16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="H16" s="7"/>
+      <c r="J16" s="10"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
     </row>
     <row r="17">
-      <c r="B17" s="2"/>
-      <c r="D17" s="3" t="s">
+      <c r="B17" s="3"/>
+      <c r="D17" s="5"/>
+      <c r="F17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="H17" s="3"/>
+      <c r="J17" s="10"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
     </row>
     <row r="18">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="9"/>
+      <c r="D18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="F18" s="8"/>
+      <c r="H18" s="7"/>
+      <c r="J18" s="10"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:H17"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Sprint Backlog.xlsx Updated code_smells_Bernardo_Atalaia from docx to txt
</commit_message>
<xml_diff>
--- a/Phase 1/Sprint1/Sprint Backlog.xlsx
+++ b/Phase 1/Sprint1/Sprint Backlog.xlsx
@@ -79,10 +79,10 @@
     <t>Martin's design patterns</t>
   </si>
   <si>
-    <t>Inacio's code smells</t>
-  </si>
-  <si>
-    <t>Inacio's design patterns (Bernardo, Carlos)</t>
+    <t>Inacio's code smells (Martin, Francisco)</t>
+  </si>
+  <si>
+    <t>Inacio's design patterns (Carlos)</t>
   </si>
   <si>
     <t>Francisco's code smells (Carlos)</t>
@@ -459,7 +459,7 @@
         <v>11</v>
       </c>
       <c r="L4" s="12">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="M4" s="12">
         <v>1.0</v>
@@ -586,10 +586,10 @@
     </row>
     <row r="15">
       <c r="B15" s="5"/>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="5"/>
+      <c r="F15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="4"/>
       <c r="H15" s="3"/>
       <c r="J15" s="13"/>
       <c r="L15" s="2"/>
@@ -644,8 +644,6 @@
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="B14:C14"/>
@@ -653,6 +651,8 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="H15:I15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D15:E15"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="B15:C15"/>

</xml_diff>

<commit_message>
Updated Sprint Backlog.xlsx Updated Scrum Board.xlsx
</commit_message>
<xml_diff>
--- a/Phase 1/Sprint1/Sprint Backlog.xlsx
+++ b/Phase 1/Sprint1/Sprint Backlog.xlsx
@@ -73,10 +73,10 @@
     <t>Carlos' design patterns</t>
   </si>
   <si>
-    <t>Martin's code smells</t>
-  </si>
-  <si>
-    <t>Martin's design patterns</t>
+    <t>Martin's code smells (Inacio)</t>
+  </si>
+  <si>
+    <t>Martin's design patterns (Inacio</t>
   </si>
   <si>
     <t>Inacio's code smells (Martin)</t>
@@ -462,7 +462,7 @@
         <v>2.0</v>
       </c>
       <c r="M4" s="10">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="N4" s="10">
         <v>1.0</v>
@@ -564,10 +564,10 @@
     </row>
     <row r="13">
       <c r="B13" s="4"/>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="4"/>
+      <c r="F13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="4"/>
       <c r="H13" s="3"/>
       <c r="J13" s="11"/>
       <c r="L13" s="2"/>
@@ -575,10 +575,10 @@
     </row>
     <row r="14">
       <c r="B14" s="9"/>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="9"/>
+      <c r="F14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="9"/>
       <c r="H14" s="8"/>
       <c r="J14" s="11"/>
       <c r="L14" s="2"/>

</xml_diff>